<commit_message>
adding email sending feature
</commit_message>
<xml_diff>
--- a/names.xlsx
+++ b/names.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\python automation\certificate automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2292EDC2-AABE-433F-ACB7-CD8C5F9E668C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69F1ACDC-E700-44EA-BDBA-AF5C265BD975}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
   <si>
     <t>Names</t>
   </si>
@@ -46,16 +46,30 @@
   </si>
   <si>
     <t>Neeraj</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>jagjit.singh21802@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -78,13 +92,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -363,50 +380,81 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.109375" customWidth="1"/>
+    <col min="2" max="2" width="28.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B6" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
+      <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B8" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{425D4036-3C42-47D8-8928-DE7F190F1E0A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>